<commit_message>
Change Generate famille1-lev1 but not used - 1|25|08|2024
</commit_message>
<xml_diff>
--- a/src/dbs/liste_categories.xlsx
+++ b/src/dbs/liste_categories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\express-la\src\dbs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619EFED0-9CC6-498C-A3F6-F0A0E11FB6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19E8CFA-8CFD-42E5-BCCD-4163C3B83D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="29040" xr2:uid="{958C5253-FACD-49B5-A96B-FF559802CB7A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{958C5253-FACD-49B5-A96B-FF559802CB7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -480,7 +480,7 @@
   <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finish all Logique famille1-lev1 et famille-ac1
</commit_message>
<xml_diff>
--- a/src/dbs/liste_categories.xlsx
+++ b/src/dbs/liste_categories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\express-la\src\dbs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19E8CFA-8CFD-42E5-BCCD-4163C3B83D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AEAB8E-C045-49EF-9AB8-AC6E3836CC64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{958C5253-FACD-49B5-A96B-FF559802CB7A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="29040" xr2:uid="{958C5253-FACD-49B5-A96B-FF559802CB7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Accessoires de levage</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>Famille AC1</t>
+  </si>
+  <si>
+    <t>Appareil de levage</t>
+  </si>
+  <si>
+    <t>Accessoire de levage</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -480,7 +489,7 @@
   <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,6 +507,9 @@
       <c r="B1" t="s">
         <v>4</v>
       </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -506,7 +518,9 @@
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -515,7 +529,9 @@
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -524,7 +540,9 @@
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -533,7 +551,9 @@
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
@@ -542,7 +562,9 @@
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -551,7 +573,9 @@
       <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>

</xml_diff>